<commit_message>
Added: Save Functionality, GameEntity & Component Classes || Updated: XLSX
We can currently:
- Run level editor;
- Open game projects;
- Add/remove scenes from project;
- Undo/redo actions;

Game Editor features:
- Menu
- Icons
- Scenes & Game Objects
- Properties & Components
- File Explorer
- Renderer
</commit_message>
<xml_diff>
--- a/Solace_Plan.xlsx
+++ b/Solace_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Solace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1ECE1D-E1FC-4F98-9A34-F353F3905A20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD8720D-25EE-4A7C-A162-BBBD8509CD5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{3A42A00D-9C57-4330-A240-180E2EBC0D59}"/>
   </bookViews>
@@ -2829,8 +2829,8 @@
   <dimension ref="A1:K211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E208" sqref="E208"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2967,7 +2967,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -2989,7 +2989,7 @@
         <v>424</v>
       </c>
       <c r="H7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -3009,7 +3009,7 @@
         <v>425</v>
       </c>
       <c r="H8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3029,7 +3029,7 @@
         <v>426</v>
       </c>
       <c r="H9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -3049,7 +3049,7 @@
         <v>427</v>
       </c>
       <c r="H10" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:11">

</xml_diff>

<commit_message>
Added: Entities System Test; Engine DLL;
</commit_message>
<xml_diff>
--- a/Solace_Plan.xlsx
+++ b/Solace_Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Solace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421D9F4-0EED-447D-8286-B01C4BEE8040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CB28BC-CFA5-4F64-B71B-5968A143ED4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3A42A00D-9C57-4330-A240-180E2EBC0D59}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="614">
   <si>
     <t>Section</t>
   </si>
@@ -1860,6 +1860,15 @@
   </si>
   <si>
     <t>110 hr 48 min</t>
+  </si>
+  <si>
+    <t>Rounded</t>
+  </si>
+  <si>
+    <t>78 hr</t>
+  </si>
+  <si>
+    <t>Progress:</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1878,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2165,9 +2174,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2205,7 +2214,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2311,7 +2320,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2453,7 +2462,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2467,22 +2476,22 @@
       <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="26.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2529,7 +2538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>13</v>
@@ -2550,7 +2559,7 @@
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="7">
         <v>1.4</v>
       </c>
@@ -2573,7 +2582,7 @@
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="14"/>
@@ -2590,7 +2599,7 @@
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -2607,7 +2616,7 @@
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="7">
         <v>1.4</v>
       </c>
@@ -2630,7 +2639,7 @@
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
@@ -2647,7 +2656,7 @@
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="17"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -2664,7 +2673,7 @@
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="7">
         <v>1.4</v>
       </c>
@@ -2685,7 +2694,7 @@
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14"/>
@@ -2702,7 +2711,7 @@
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="17"/>
       <c r="B11" s="18" t="s">
         <v>29</v>
@@ -2721,7 +2730,7 @@
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="7">
         <v>1.4</v>
       </c>
@@ -2744,7 +2753,7 @@
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
@@ -2761,7 +2770,7 @@
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="17"/>
       <c r="B14" s="18" t="s">
         <v>27</v>
@@ -2780,7 +2789,7 @@
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="7">
         <v>1.4</v>
       </c>
@@ -2801,7 +2810,7 @@
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14"/>
@@ -2818,7 +2827,7 @@
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -2843,27 +2852,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F24280-107B-4A2D-B2C2-14E940A88640}">
-  <dimension ref="A1:J211"/>
+  <dimension ref="A1:K211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A206" sqref="A206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="34" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="32" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="32" customFormat="1">
       <c r="A1" s="31" t="s">
         <v>30</v>
       </c>
@@ -2894,8 +2904,11 @@
       <c r="J1" s="30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="30" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>31</v>
@@ -2910,8 +2923,9 @@
       <c r="J2" s="24" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>33</v>
@@ -2924,8 +2938,9 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>32</v>
@@ -2938,8 +2953,9 @@
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="33">
         <v>1</v>
       </c>
@@ -2964,8 +2980,11 @@
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="29">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="33">
         <v>2</v>
       </c>
@@ -2990,8 +3009,11 @@
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="33">
         <v>3</v>
       </c>
@@ -3013,8 +3035,11 @@
       <c r="H7" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="33">
         <v>4</v>
       </c>
@@ -3036,8 +3061,11 @@
       <c r="H8" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="33">
         <v>5</v>
       </c>
@@ -3059,8 +3087,11 @@
       <c r="H9" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="29">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="33">
         <v>6</v>
       </c>
@@ -3082,8 +3113,11 @@
       <c r="H10" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="29">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="33">
         <v>7</v>
       </c>
@@ -3105,8 +3139,11 @@
       <c r="H11" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="29">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="33">
         <v>8</v>
       </c>
@@ -3128,8 +3165,11 @@
       <c r="H12" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="29">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="33">
         <v>9</v>
       </c>
@@ -3146,10 +3186,13 @@
         <v>429</v>
       </c>
       <c r="H13" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+      <c r="K13" s="29">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="33">
         <v>10</v>
       </c>
@@ -3166,10 +3209,13 @@
         <v>430</v>
       </c>
       <c r="H14" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+      <c r="K14" s="29">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="33">
         <v>11</v>
       </c>
@@ -3186,10 +3232,13 @@
         <v>431</v>
       </c>
       <c r="H15" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+      <c r="K15" s="29">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="33">
         <v>12</v>
       </c>
@@ -3208,8 +3257,11 @@
       <c r="H16" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K16" s="29">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="33">
         <v>13</v>
       </c>
@@ -3226,8 +3278,11 @@
       <c r="H17" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K17" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="33">
         <v>14</v>
       </c>
@@ -3246,8 +3301,11 @@
       <c r="H18" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K18" s="29">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="33">
         <v>15</v>
       </c>
@@ -3266,8 +3324,11 @@
       <c r="H19" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K19" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="33">
         <v>16</v>
       </c>
@@ -3286,8 +3347,11 @@
       <c r="H20" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K20" s="29">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="33">
         <v>17</v>
       </c>
@@ -3306,8 +3370,11 @@
       <c r="H21" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K21" s="29">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="33">
         <v>18</v>
       </c>
@@ -3326,8 +3393,11 @@
       <c r="H22" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K22" s="29">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="33">
         <v>19</v>
       </c>
@@ -3346,8 +3416,11 @@
       <c r="H23" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K23" s="29">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="33">
         <v>20</v>
       </c>
@@ -3364,8 +3437,11 @@
       <c r="H24" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K24" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="33">
         <v>21</v>
       </c>
@@ -3384,8 +3460,11 @@
       <c r="H25" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K25" s="29">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="33">
         <v>22</v>
       </c>
@@ -3404,8 +3483,11 @@
       <c r="H26" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K26" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="33">
         <v>23</v>
       </c>
@@ -3424,8 +3506,11 @@
       <c r="H27" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K27" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="33">
         <v>24</v>
       </c>
@@ -3444,8 +3529,11 @@
       <c r="H28" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K28" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="33">
         <v>25</v>
       </c>
@@ -3464,8 +3552,11 @@
       <c r="H29" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K29" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="33">
         <v>26</v>
       </c>
@@ -3484,8 +3575,11 @@
       <c r="H30" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K30" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="33">
         <v>27</v>
       </c>
@@ -3504,8 +3598,11 @@
       <c r="H31" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K31" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="33">
         <v>28</v>
       </c>
@@ -3522,8 +3619,11 @@
       <c r="H32" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K32" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="33">
         <v>29</v>
       </c>
@@ -3542,8 +3642,11 @@
       <c r="H33" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K33" s="29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="33">
         <v>30</v>
       </c>
@@ -3562,8 +3665,11 @@
       <c r="H34" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K34" s="29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="33">
         <v>31</v>
       </c>
@@ -3582,8 +3688,11 @@
       <c r="H35" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K35" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="33">
         <v>32</v>
       </c>
@@ -3602,8 +3711,11 @@
       <c r="H36" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K36" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="33">
         <v>33</v>
       </c>
@@ -3622,8 +3734,11 @@
       <c r="H37" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K37" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="33">
         <v>34</v>
       </c>
@@ -3642,8 +3757,11 @@
       <c r="H38" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K38" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="33">
         <v>35</v>
       </c>
@@ -3662,8 +3780,11 @@
       <c r="H39" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K39" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="33">
         <v>36</v>
       </c>
@@ -3682,8 +3803,11 @@
       <c r="H40" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K40" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="33">
         <v>37</v>
       </c>
@@ -3702,8 +3826,11 @@
       <c r="H41" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K41" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="33">
         <v>38</v>
       </c>
@@ -3722,8 +3849,11 @@
       <c r="H42" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K42" s="29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="33">
         <v>39</v>
       </c>
@@ -3742,8 +3872,11 @@
       <c r="H43" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K43" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="33">
         <v>40</v>
       </c>
@@ -3762,8 +3895,11 @@
       <c r="H44" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K44" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="33">
         <v>41</v>
       </c>
@@ -3782,8 +3918,11 @@
       <c r="H45" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K45" s="29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="33">
         <v>42</v>
       </c>
@@ -3802,8 +3941,11 @@
       <c r="H46" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K46" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="33">
         <v>43</v>
       </c>
@@ -3822,8 +3964,11 @@
       <c r="H47" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K47" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="33">
         <v>44</v>
       </c>
@@ -3842,8 +3987,11 @@
       <c r="H48" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K48" s="29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="33">
         <v>45</v>
       </c>
@@ -3862,8 +4010,11 @@
       <c r="H49" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K49" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="33">
         <v>46</v>
       </c>
@@ -3882,8 +4033,11 @@
       <c r="H50" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K50" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="33">
         <v>47</v>
       </c>
@@ -3902,8 +4056,11 @@
       <c r="H51" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K51" s="29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="33">
         <v>48</v>
       </c>
@@ -3922,8 +4079,11 @@
       <c r="H52" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K52" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="33">
         <v>49</v>
       </c>
@@ -3942,8 +4102,11 @@
       <c r="H53" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K53" s="29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="33">
         <v>50</v>
       </c>
@@ -3962,8 +4125,11 @@
       <c r="H54" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K54" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="33">
         <v>51</v>
       </c>
@@ -3982,8 +4148,11 @@
       <c r="H55" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K55" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="33">
         <v>52</v>
       </c>
@@ -4002,8 +4171,11 @@
       <c r="H56" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K56" s="29">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="33">
         <v>53</v>
       </c>
@@ -4022,8 +4194,11 @@
       <c r="H57" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K57" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="33">
         <v>54</v>
       </c>
@@ -4042,8 +4217,11 @@
       <c r="H58" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K58" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="33">
         <v>55</v>
       </c>
@@ -4062,8 +4240,11 @@
       <c r="H59" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K59" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="33">
         <v>56</v>
       </c>
@@ -4082,8 +4263,11 @@
       <c r="H60" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K60" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="33">
         <v>57</v>
       </c>
@@ -4102,8 +4286,11 @@
       <c r="H61" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K61" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="33">
         <v>58</v>
       </c>
@@ -4122,8 +4309,11 @@
       <c r="H62" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K62" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="33">
         <v>59</v>
       </c>
@@ -4142,8 +4332,11 @@
       <c r="H63" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K63" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="33">
         <v>60</v>
       </c>
@@ -4162,8 +4355,11 @@
       <c r="H64" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K64" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="33">
         <v>61</v>
       </c>
@@ -4182,8 +4378,11 @@
       <c r="H65" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K65" s="29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="33">
         <v>62</v>
       </c>
@@ -4202,8 +4401,11 @@
       <c r="H66" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K66" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="33">
         <v>63</v>
       </c>
@@ -4222,8 +4424,11 @@
       <c r="H67" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K67" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" s="33">
         <v>64</v>
       </c>
@@ -4242,8 +4447,11 @@
       <c r="H68" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K68" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" s="33">
         <v>65</v>
       </c>
@@ -4262,8 +4470,11 @@
       <c r="H69" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K69" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="33">
         <v>66</v>
       </c>
@@ -4282,8 +4493,11 @@
       <c r="H70" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K70" s="29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" s="33">
         <v>67</v>
       </c>
@@ -4302,8 +4516,11 @@
       <c r="H71" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K71" s="29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="33">
         <v>68</v>
       </c>
@@ -4322,8 +4539,11 @@
       <c r="H72" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K72" s="29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="33">
         <v>69</v>
       </c>
@@ -4342,8 +4562,11 @@
       <c r="H73" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K73" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="33">
         <v>70</v>
       </c>
@@ -4362,8 +4585,11 @@
       <c r="H74" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K74" s="29">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="33">
         <v>71</v>
       </c>
@@ -4382,8 +4608,11 @@
       <c r="H75" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K75" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="33">
         <v>72</v>
       </c>
@@ -4402,8 +4631,11 @@
       <c r="H76" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K76" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="33">
         <v>73</v>
       </c>
@@ -4422,8 +4654,11 @@
       <c r="H77" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K77" s="29">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="33">
         <v>74</v>
       </c>
@@ -4442,8 +4677,11 @@
       <c r="H78" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K78" s="29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="33">
         <v>75</v>
       </c>
@@ -4462,8 +4700,11 @@
       <c r="H79" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K79" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="33">
         <v>76</v>
       </c>
@@ -4482,8 +4723,11 @@
       <c r="H80" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K80" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" s="33">
         <v>77</v>
       </c>
@@ -4502,8 +4746,11 @@
       <c r="H81" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K81" s="29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" s="33">
         <v>78</v>
       </c>
@@ -4522,8 +4769,11 @@
       <c r="H82" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K82" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="33">
         <v>79</v>
       </c>
@@ -4542,8 +4792,11 @@
       <c r="H83" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K83" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="33">
         <v>80</v>
       </c>
@@ -4562,8 +4815,11 @@
       <c r="H84" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K84" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" s="33">
         <v>81</v>
       </c>
@@ -4582,8 +4838,11 @@
       <c r="H85" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K85" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" s="33">
         <v>82</v>
       </c>
@@ -4602,8 +4861,11 @@
       <c r="H86" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K86" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" s="33">
         <v>83</v>
       </c>
@@ -4622,8 +4884,11 @@
       <c r="H87" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K87" s="29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" s="33">
         <v>84</v>
       </c>
@@ -4642,8 +4907,11 @@
       <c r="H88" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K88" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" s="33">
         <v>85</v>
       </c>
@@ -4662,8 +4930,11 @@
       <c r="H89" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K89" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" s="33">
         <v>86</v>
       </c>
@@ -4682,8 +4953,11 @@
       <c r="H90" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K90" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" s="33">
         <v>87</v>
       </c>
@@ -4702,8 +4976,11 @@
       <c r="H91" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K91" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" s="33">
         <v>88</v>
       </c>
@@ -4722,8 +4999,11 @@
       <c r="H92" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K92" s="29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" s="33">
         <v>89</v>
       </c>
@@ -4742,8 +5022,11 @@
       <c r="H93" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K93" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" s="33">
         <v>90</v>
       </c>
@@ -4762,8 +5045,11 @@
       <c r="H94" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K94" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" s="33">
         <v>91</v>
       </c>
@@ -4782,8 +5068,11 @@
       <c r="H95" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K95" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" s="33">
         <v>92</v>
       </c>
@@ -4802,8 +5091,11 @@
       <c r="H96" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K96" s="29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" s="33">
         <v>93</v>
       </c>
@@ -4822,8 +5114,11 @@
       <c r="H97" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K97" s="29">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" s="33">
         <v>94</v>
       </c>
@@ -4842,8 +5137,11 @@
       <c r="H98" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K98" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" s="33">
         <v>95</v>
       </c>
@@ -4862,8 +5160,11 @@
       <c r="H99" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K99" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" s="33">
         <v>96</v>
       </c>
@@ -4882,8 +5183,11 @@
       <c r="H100" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K100" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101" s="33">
         <v>97</v>
       </c>
@@ -4902,8 +5206,11 @@
       <c r="H101" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K101" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" s="33">
         <v>98</v>
       </c>
@@ -4922,8 +5229,11 @@
       <c r="H102" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K102" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" s="33">
         <v>99</v>
       </c>
@@ -4942,8 +5252,11 @@
       <c r="H103" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K103" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" s="33">
         <v>100</v>
       </c>
@@ -4962,8 +5275,11 @@
       <c r="H104" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K104" s="29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" s="33">
         <v>101</v>
       </c>
@@ -4982,8 +5298,11 @@
       <c r="H105" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K105" s="29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" s="33">
         <v>102</v>
       </c>
@@ -5002,8 +5321,11 @@
       <c r="H106" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K106" s="29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" s="33">
         <v>103</v>
       </c>
@@ -5022,8 +5344,11 @@
       <c r="H107" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K107" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" s="33">
         <v>104</v>
       </c>
@@ -5042,8 +5367,11 @@
       <c r="H108" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K108" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" s="33">
         <v>105</v>
       </c>
@@ -5062,8 +5390,11 @@
       <c r="H109" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K109" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110" s="33">
         <v>106</v>
       </c>
@@ -5082,8 +5413,11 @@
       <c r="H110" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K110" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111" s="33">
         <v>107</v>
       </c>
@@ -5102,8 +5436,11 @@
       <c r="H111" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K111" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112" s="33">
         <v>108</v>
       </c>
@@ -5122,8 +5459,11 @@
       <c r="H112" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K112" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113" s="33">
         <v>109</v>
       </c>
@@ -5142,8 +5482,11 @@
       <c r="H113" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K113" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114" s="33">
         <v>110</v>
       </c>
@@ -5162,8 +5505,11 @@
       <c r="H114" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K114" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115" s="33">
         <v>111</v>
       </c>
@@ -5182,8 +5528,11 @@
       <c r="H115" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K115" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116" s="33">
         <v>112</v>
       </c>
@@ -5202,8 +5551,11 @@
       <c r="H116" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K116" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" s="33">
         <v>113</v>
       </c>
@@ -5222,8 +5574,11 @@
       <c r="H117" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K117" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118" s="33">
         <v>114</v>
       </c>
@@ -5242,8 +5597,11 @@
       <c r="H118" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K118" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" s="33">
         <v>115</v>
       </c>
@@ -5262,8 +5620,11 @@
       <c r="H119" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K119" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120" s="33">
         <v>116</v>
       </c>
@@ -5282,8 +5643,11 @@
       <c r="H120" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K120" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121" s="33">
         <v>117</v>
       </c>
@@ -5302,8 +5666,11 @@
       <c r="H121" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K121" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" s="33">
         <v>118</v>
       </c>
@@ -5322,8 +5689,11 @@
       <c r="H122" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K122" s="29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" s="33">
         <v>119</v>
       </c>
@@ -5342,8 +5712,11 @@
       <c r="H123" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K123" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" s="33">
         <v>120</v>
       </c>
@@ -5362,8 +5735,11 @@
       <c r="H124" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K124" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125" s="33">
         <v>121</v>
       </c>
@@ -5382,8 +5758,11 @@
       <c r="H125" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K125" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126" s="33">
         <v>122</v>
       </c>
@@ -5402,8 +5781,11 @@
       <c r="H126" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K126" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127" s="33">
         <v>123</v>
       </c>
@@ -5422,8 +5804,11 @@
       <c r="H127" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K127" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128" s="33">
         <v>124</v>
       </c>
@@ -5442,8 +5827,11 @@
       <c r="H128" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K128" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
       <c r="A129" s="33">
         <v>125</v>
       </c>
@@ -5462,8 +5850,11 @@
       <c r="H129" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K129" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
       <c r="A130" s="33">
         <v>126</v>
       </c>
@@ -5482,8 +5873,11 @@
       <c r="H130" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K130" s="29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
       <c r="A131" s="33">
         <v>127</v>
       </c>
@@ -5502,8 +5896,11 @@
       <c r="H131" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K131" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
       <c r="A132" s="33">
         <v>128</v>
       </c>
@@ -5522,8 +5919,11 @@
       <c r="H132" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K132" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
       <c r="A133" s="33">
         <v>129</v>
       </c>
@@ -5542,8 +5942,11 @@
       <c r="H133" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K133" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
       <c r="A134" s="33">
         <v>130</v>
       </c>
@@ -5562,8 +5965,11 @@
       <c r="H134" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K134" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
       <c r="A135" s="33">
         <v>131</v>
       </c>
@@ -5582,8 +5988,11 @@
       <c r="H135" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K135" s="29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
       <c r="A136" s="33">
         <v>132</v>
       </c>
@@ -5602,8 +6011,11 @@
       <c r="H136" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K136" s="29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
       <c r="A137" s="33">
         <v>133</v>
       </c>
@@ -5622,8 +6034,11 @@
       <c r="H137" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K137" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138" s="33">
         <v>134</v>
       </c>
@@ -5642,8 +6057,11 @@
       <c r="H138" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K138" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139" s="33">
         <v>135</v>
       </c>
@@ -5662,8 +6080,11 @@
       <c r="H139" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K139" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
       <c r="A140" s="33">
         <v>136</v>
       </c>
@@ -5682,8 +6103,11 @@
       <c r="H140" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K140" s="29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
       <c r="A141" s="33">
         <v>137</v>
       </c>
@@ -5702,8 +6126,11 @@
       <c r="H141" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K141" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
       <c r="A142" s="33">
         <v>138</v>
       </c>
@@ -5722,8 +6149,11 @@
       <c r="H142" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K142" s="29">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11">
       <c r="A143" s="33">
         <v>139</v>
       </c>
@@ -5742,8 +6172,11 @@
       <c r="H143" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K143" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
       <c r="A144" s="33">
         <v>140</v>
       </c>
@@ -5762,8 +6195,11 @@
       <c r="H144" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K144" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11">
       <c r="A145" s="33">
         <v>141</v>
       </c>
@@ -5782,8 +6218,11 @@
       <c r="H145" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K145" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11">
       <c r="A146" s="33">
         <v>142</v>
       </c>
@@ -5802,8 +6241,11 @@
       <c r="H146" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K146" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11">
       <c r="A147" s="33">
         <v>143</v>
       </c>
@@ -5822,8 +6264,11 @@
       <c r="H147" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K147" s="29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11">
       <c r="A148" s="33">
         <v>144</v>
       </c>
@@ -5842,8 +6287,11 @@
       <c r="H148" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K148" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11">
       <c r="A149" s="33">
         <v>145</v>
       </c>
@@ -5862,8 +6310,11 @@
       <c r="H149" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K149" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11">
       <c r="A150" s="33">
         <v>146</v>
       </c>
@@ -5882,8 +6333,11 @@
       <c r="H150" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K150" s="29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11">
       <c r="A151" s="33">
         <v>147</v>
       </c>
@@ -5902,8 +6356,11 @@
       <c r="H151" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K151" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11">
       <c r="A152" s="33">
         <v>148</v>
       </c>
@@ -5922,8 +6379,11 @@
       <c r="H152" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K152" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11">
       <c r="A153" s="33">
         <v>149</v>
       </c>
@@ -5942,8 +6402,11 @@
       <c r="H153" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K153" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11">
       <c r="A154" s="33">
         <v>150</v>
       </c>
@@ -5962,8 +6425,11 @@
       <c r="H154" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K154" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11">
       <c r="A155" s="33">
         <v>151</v>
       </c>
@@ -5982,8 +6448,11 @@
       <c r="H155" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K155" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11">
       <c r="A156" s="33">
         <v>152</v>
       </c>
@@ -6002,8 +6471,11 @@
       <c r="H156" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K156" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11">
       <c r="A157" s="33">
         <v>153</v>
       </c>
@@ -6022,8 +6494,11 @@
       <c r="H157" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K157" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11">
       <c r="A158" s="33">
         <v>154</v>
       </c>
@@ -6042,8 +6517,11 @@
       <c r="H158" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K158" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11">
       <c r="A159" s="33">
         <v>155</v>
       </c>
@@ -6062,8 +6540,11 @@
       <c r="H159" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K159" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11">
       <c r="A160" s="33">
         <v>156</v>
       </c>
@@ -6082,8 +6563,11 @@
       <c r="H160" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K160" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
       <c r="A161" s="33">
         <v>157</v>
       </c>
@@ -6102,8 +6586,11 @@
       <c r="H161" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K161" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
       <c r="A162" s="33">
         <v>158</v>
       </c>
@@ -6122,8 +6609,11 @@
       <c r="H162" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K162" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
       <c r="A163" s="33">
         <v>159</v>
       </c>
@@ -6142,8 +6632,11 @@
       <c r="H163" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K163" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11">
       <c r="A164" s="33">
         <v>160</v>
       </c>
@@ -6162,8 +6655,11 @@
       <c r="H164" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K164" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11">
       <c r="A165" s="33">
         <v>161</v>
       </c>
@@ -6182,8 +6678,11 @@
       <c r="H165" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K165" s="29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11">
       <c r="A166" s="33">
         <v>162</v>
       </c>
@@ -6202,8 +6701,11 @@
       <c r="H166" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K166" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11">
       <c r="A167" s="33">
         <v>163</v>
       </c>
@@ -6222,8 +6724,11 @@
       <c r="H167" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K167" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11">
       <c r="A168" s="33">
         <v>164</v>
       </c>
@@ -6242,8 +6747,11 @@
       <c r="H168" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K168" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11">
       <c r="A169" s="33">
         <v>165</v>
       </c>
@@ -6262,8 +6770,11 @@
       <c r="H169" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K169" s="29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11">
       <c r="A170" s="33">
         <v>166</v>
       </c>
@@ -6282,8 +6793,11 @@
       <c r="H170" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K170" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11">
       <c r="A171" s="33">
         <v>167</v>
       </c>
@@ -6302,8 +6816,11 @@
       <c r="H171" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K171" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11">
       <c r="A172" s="33">
         <v>168</v>
       </c>
@@ -6322,8 +6839,11 @@
       <c r="H172" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K172" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11">
       <c r="A173" s="33">
         <v>169</v>
       </c>
@@ -6342,8 +6862,11 @@
       <c r="H173" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K173" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11">
       <c r="A174" s="33">
         <v>170</v>
       </c>
@@ -6362,8 +6885,11 @@
       <c r="H174" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K174" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
       <c r="A175" s="33">
         <v>171</v>
       </c>
@@ -6382,8 +6908,11 @@
       <c r="H175" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K175" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11">
       <c r="A176" s="33">
         <v>172</v>
       </c>
@@ -6402,8 +6931,11 @@
       <c r="H176" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K176" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11">
       <c r="A177" s="33">
         <v>173</v>
       </c>
@@ -6422,8 +6954,11 @@
       <c r="H177" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K177" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11">
       <c r="A178" s="33">
         <v>174</v>
       </c>
@@ -6442,8 +6977,11 @@
       <c r="H178" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K178" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11">
       <c r="A179" s="33">
         <v>175</v>
       </c>
@@ -6462,8 +7000,11 @@
       <c r="H179" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K179" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11">
       <c r="A180" s="33">
         <v>176</v>
       </c>
@@ -6482,8 +7023,11 @@
       <c r="H180" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K180" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11">
       <c r="A181" s="33">
         <v>177</v>
       </c>
@@ -6502,8 +7046,11 @@
       <c r="H181" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K181" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11">
       <c r="A182" s="33">
         <v>178</v>
       </c>
@@ -6522,8 +7069,11 @@
       <c r="H182" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K182" s="29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11">
       <c r="A183" s="33">
         <v>179</v>
       </c>
@@ -6542,8 +7092,11 @@
       <c r="H183" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K183" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11">
       <c r="A184" s="33">
         <v>180</v>
       </c>
@@ -6562,8 +7115,11 @@
       <c r="H184" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K184" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11">
       <c r="A185" s="33">
         <v>181</v>
       </c>
@@ -6582,8 +7138,11 @@
       <c r="H185" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K185" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11">
       <c r="A186" s="33">
         <v>182</v>
       </c>
@@ -6602,8 +7161,11 @@
       <c r="H186" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K186" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11">
       <c r="A187" s="33">
         <v>183</v>
       </c>
@@ -6622,8 +7184,11 @@
       <c r="H187" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K187" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11">
       <c r="A188" s="33">
         <v>184</v>
       </c>
@@ -6642,8 +7207,11 @@
       <c r="H188" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K188" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11">
       <c r="A189" s="33">
         <v>185</v>
       </c>
@@ -6662,8 +7230,11 @@
       <c r="H189" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K189" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11">
       <c r="A190" s="33">
         <v>186</v>
       </c>
@@ -6682,8 +7253,11 @@
       <c r="H190" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K190" s="29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11">
       <c r="A191" s="33">
         <v>187</v>
       </c>
@@ -6702,8 +7276,11 @@
       <c r="H191" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K191" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11">
       <c r="A192" s="33">
         <v>188</v>
       </c>
@@ -6722,8 +7299,11 @@
       <c r="H192" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K192" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11">
       <c r="A193" s="33">
         <v>189</v>
       </c>
@@ -6742,8 +7322,11 @@
       <c r="H193" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K193" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11">
       <c r="A194" s="33">
         <v>190</v>
       </c>
@@ -6762,8 +7345,11 @@
       <c r="H194" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K194" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11">
       <c r="A195" s="33">
         <v>191</v>
       </c>
@@ -6782,8 +7368,11 @@
       <c r="H195" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K195" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11">
       <c r="A196" s="33">
         <v>192</v>
       </c>
@@ -6802,8 +7391,11 @@
       <c r="H196" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K196" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11">
       <c r="A197" s="33">
         <v>193</v>
       </c>
@@ -6822,8 +7414,11 @@
       <c r="H197" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K197" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11">
       <c r="A198" s="33">
         <v>194</v>
       </c>
@@ -6842,8 +7437,11 @@
       <c r="H198" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K198" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11">
       <c r="A199" s="33">
         <v>195</v>
       </c>
@@ -6862,8 +7460,11 @@
       <c r="H199" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K199" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11">
       <c r="A200" s="33">
         <v>196</v>
       </c>
@@ -6882,8 +7483,11 @@
       <c r="H200" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K200" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11">
       <c r="A201" s="33">
         <v>197</v>
       </c>
@@ -6902,8 +7506,11 @@
       <c r="H201" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K201" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11">
       <c r="A202" s="33">
         <v>198</v>
       </c>
@@ -6922,8 +7529,11 @@
       <c r="H202" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K202" s="29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11">
       <c r="A203" s="33">
         <v>199</v>
       </c>
@@ -6942,8 +7552,11 @@
       <c r="H203" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K203" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11">
       <c r="A204" s="33">
         <v>200</v>
       </c>
@@ -6962,35 +7575,55 @@
       <c r="H204" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K204" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11">
       <c r="D205" s="40"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D206" s="40"/>
+    <row r="206" spans="1:11">
+      <c r="D206" s="29">
+        <v>280734</v>
+      </c>
       <c r="E206" s="29" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D207" s="40"/>
+      <c r="G206" t="s">
+        <v>613</v>
+      </c>
+      <c r="H206">
+        <f>SUMIFS(K5:K204, H5:H204, "Complete")</f>
+        <v>535</v>
+      </c>
+      <c r="K206">
+        <f>SUM(K5:K204)</f>
+        <v>4677</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11">
+      <c r="D207" s="29">
+        <v>4679</v>
+      </c>
       <c r="E207" s="29" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D208" s="40"/>
+    <row r="208" spans="1:11">
+      <c r="D208" s="29" t="s">
+        <v>612</v>
+      </c>
       <c r="E208" s="29" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="4:4">
       <c r="D209" s="40"/>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="4:4">
       <c r="D210" s="40"/>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="4:4">
       <c r="D211" s="40"/>
     </row>
   </sheetData>
@@ -7015,12 +7648,12 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3">
       <c r="B2" s="19" t="s">
         <v>18</v>
       </c>
@@ -7028,7 +7661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" s="20" t="s">
         <v>20</v>
       </c>
@@ -7036,7 +7669,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" s="21" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Added: Menu Navigation Animation || Updated: Editor UI
Easing function added for navigation between OpenProject & NewProject.
</commit_message>
<xml_diff>
--- a/Solace_Plan.xlsx
+++ b/Solace_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Solace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31934E92-113B-40ED-B834-A437BB180F67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DDA45D-A974-471F-8B7E-A4736B81AF29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3A42A00D-9C57-4330-A240-180E2EBC0D59}"/>
   </bookViews>
@@ -2856,7 +2856,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3263,8 +3263,11 @@
       <c r="E16" s="27" t="s">
         <v>432</v>
       </c>
+      <c r="F16" s="34">
+        <v>45707</v>
+      </c>
       <c r="H16" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K16" s="29">
         <v>54</v>
@@ -3285,7 +3288,7 @@
         <v>433</v>
       </c>
       <c r="H17" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="K17" s="29">
         <v>5</v>
@@ -7603,7 +7606,7 @@
       </c>
       <c r="H206">
         <f>SUMIFS(K5:K204, H5:H204, "Complete")</f>
-        <v>618</v>
+        <v>672</v>
       </c>
       <c r="K206">
         <f>SUM(K5:K204)</f>

</xml_diff>

<commit_message>
Updated: Template & Showcase Images || Fixed: LoggerView Bug
</commit_message>
<xml_diff>
--- a/Solace_Plan.xlsx
+++ b/Solace_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Solace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57047AC-7B55-4668-9066-A35D76966522}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3CC93D-8363-47DF-B458-4CE80C90A452}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="7644" activeTab="1" xr2:uid="{3A42A00D-9C57-4330-A240-180E2EBC0D59}"/>
   </bookViews>
@@ -2856,7 +2856,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3310,8 +3310,11 @@
       <c r="E18" s="27" t="s">
         <v>434</v>
       </c>
+      <c r="F18" s="34">
+        <v>45714</v>
+      </c>
       <c r="H18" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K18" s="29">
         <v>42</v>
@@ -3334,7 +3337,7 @@
         <v>435</v>
       </c>
       <c r="H19" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="K19" s="29">
         <v>49</v>
@@ -7606,7 +7609,7 @@
       </c>
       <c r="H206">
         <f>SUMIFS(K5:K204, H5:H204, "Complete")</f>
-        <v>677</v>
+        <v>719</v>
       </c>
       <c r="K206">
         <f>SUM(K5:K204)</f>

</xml_diff>